<commit_message>
added more SonarLint solutions
</commit_message>
<xml_diff>
--- a/03_PizzaShop/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/03_PizzaShop/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Documents\VVSS\VVSSPizzaShop\03_PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891C3307-61A6-4061-A9DB-688702397FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938058CF-21C2-4641-AC24-DB90622BB1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="100">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -524,6 +524,53 @@
   </si>
   <si>
     <t>Pizza types and prices aren't specified</t>
+  </si>
+  <si>
+    <t>PaymentAlert/46</t>
+  </si>
+  <si>
+    <t>Optional value should only be accessed after calling isPresent()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (result.get() == cardPayment) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  if(result.isPresent()) {
+            if (result.get() == cardPayment) {..}}</t>
+  </si>
+  <si>
+    <t>PaymentRepository/3</t>
+  </si>
+  <si>
+    <t>Unnecessary imports should be removed</t>
+  </si>
+  <si>
+    <t>import javafx.collections.ObservableList;</t>
+  </si>
+  <si>
+    <t>PaymentRepository/30</t>
+  </si>
+  <si>
+    <t>Catches should be combined</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>KitchenGUI/28</t>
+  </si>
+  <si>
+    <t>Anonymous inner classes containing only one method should become lambdas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        stage.setOnCloseRequest(new EventHandler&lt;WindowEvent&gt;() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        stage.setOnCloseRequest(event -&gt; {..}</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1847,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -2166,8 +2213,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -2175,7 +2222,7 @@
     <col min="1" max="1" width="8.90625" style="6"/>
     <col min="2" max="2" width="12.1796875" style="6" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32.90625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="65.54296875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.6328125" style="6" customWidth="1"/>
     <col min="6" max="6" width="52.54296875" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.90625" style="6"/>
@@ -2396,45 +2443,75 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="29">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="C16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="29">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="72.5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="29">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="3">

</xml_diff>